<commit_message>
Changes for new board and setting Solar current baseline
</commit_message>
<xml_diff>
--- a/Voltage Drop calcs.xlsx
+++ b/Voltage Drop calcs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4f761af6c3887222/Documents/Arduino/greenHouse/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4f761af6c3887222/Documents/Arduino/Greenhouse/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="8_{A6A8BC29-97B7-45FA-BEF7-5C00A8988C7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DFA6A1A9-FC00-4152-B0CA-C3673A290047}"/>
+  <xr:revisionPtr revIDLastSave="91" documentId="8_{A6A8BC29-97B7-45FA-BEF7-5C00A8988C7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DA0B26A6-6632-4EAC-9442-127B4E3752DE}"/>
   <bookViews>
-    <workbookView xWindow="5055" yWindow="570" windowWidth="21600" windowHeight="13545" xr2:uid="{B5AC4ED2-AFA6-44C5-A5F0-535C8E4C1FA9}"/>
+    <workbookView xWindow="10995" yWindow="885" windowWidth="28260" windowHeight="15345" xr2:uid="{B5AC4ED2-AFA6-44C5-A5F0-535C8E4C1FA9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -408,15 +408,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF371F63-87FF-4ABD-88EE-A7916358AB1A}">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -436,34 +436,87 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>4700</v>
       </c>
       <c r="B2">
-        <v>10000</v>
+        <f>4700*2</f>
+        <v>9400</v>
       </c>
       <c r="D2">
-        <v>5.2</v>
+        <v>5</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <f>((B2/(A2+B2))*D2)-A7</f>
-        <v>3.5374149659863945</v>
+        <f>((B2/(A2+B2))*D2)-E2</f>
+        <v>3.333333333333333</v>
       </c>
       <c r="H2">
         <f>D2/(A2+B2)</f>
-        <v>3.5374149659863946E-4</v>
+        <v>3.5460992907801421E-4</v>
       </c>
       <c r="K2">
         <f>A2+B2</f>
-        <v>14700</v>
+        <v>14100</v>
       </c>
       <c r="L2">
         <f>B2/K2</f>
-        <v>0.68027210884353739</v>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="N2">
+        <f>F2/2</f>
+        <v>1.6666666666666665</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f>47000*2</f>
+        <v>94000</v>
+      </c>
+      <c r="B4">
+        <f>10000*2</f>
+        <v>20000</v>
+      </c>
+      <c r="D4">
+        <v>19</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <f>((B4/(A4+B4))*D4)-E4</f>
+        <v>3.333333333333333</v>
+      </c>
+      <c r="H4">
+        <f>D4/(A4+B4)</f>
+        <v>1.6666666666666666E-4</v>
+      </c>
+      <c r="K4">
+        <f>A4+B4</f>
+        <v>114000</v>
+      </c>
+      <c r="L4">
+        <f>B4/K4</f>
+        <v>0.17543859649122806</v>
+      </c>
+      <c r="N4">
+        <f>F4/2</f>
+        <v>1.6666666666666665</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H7">
+        <f>2*H2+H4</f>
+        <v>8.7588652482269505E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <f>19/4096</f>
+        <v>4.638671875E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>